<commit_message>
Changed some items to dicts
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -466,7 +466,7 @@
         <v>95.27974700927734</v>
       </c>
       <c r="D2" t="n">
-        <v>10.68385142857143</v>
+        <v>10.65735728007408</v>
       </c>
     </row>
     <row r="3">
@@ -480,7 +480,7 @@
         <v>131.8361968994141</v>
       </c>
       <c r="D3" t="n">
-        <v>0.81202</v>
+        <v>0.8010256137157513</v>
       </c>
     </row>
     <row r="4">
@@ -494,7 +494,7 @@
         <v>70.85282897949219</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2</v>
+        <v>0.002783467301713101</v>
       </c>
     </row>
     <row r="5">
@@ -508,7 +508,7 @@
         <v>71.70697021484375</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1</v>
+        <v>0.002750767903118707</v>
       </c>
     </row>
     <row r="6">
@@ -522,7 +522,7 @@
         <v>76.90805053710938</v>
       </c>
       <c r="D6" t="n">
-        <v>0.06666666666666667</v>
+        <v>0.002567128796333255</v>
       </c>
     </row>
     <row r="7">
@@ -536,7 +536,7 @@
         <v>78.24656677246094</v>
       </c>
       <c r="D7" t="n">
-        <v>0.05</v>
+        <v>0.002523768639394259</v>
       </c>
     </row>
     <row r="8">
@@ -550,7 +550,7 @@
         <v>78.48947143554688</v>
       </c>
       <c r="D8" t="n">
-        <v>0.04000000000000001</v>
+        <v>0.002516056483809528</v>
       </c>
     </row>
     <row r="9">
@@ -564,7 +564,7 @@
         <v>93.44825744628906</v>
       </c>
       <c r="D9" t="n">
-        <v>0.03333333333333333</v>
+        <v>0.002117561566593605</v>
       </c>
     </row>
     <row r="10">
@@ -578,7 +578,7 @@
         <v>103.6337432861328</v>
       </c>
       <c r="D10" t="n">
-        <v>0.025</v>
+        <v>0.001911429274331488</v>
       </c>
     </row>
     <row r="11">
@@ -592,7 +592,7 @@
         <v>106.6675033569336</v>
       </c>
       <c r="D11" t="n">
-        <v>0.02222222222222222</v>
+        <v>0.001857570703919553</v>
       </c>
     </row>
     <row r="12">
@@ -606,7 +606,7 @@
         <v>110.8966445922852</v>
       </c>
       <c r="D12" t="n">
-        <v>0.02</v>
+        <v>0.001787363693779511</v>
       </c>
     </row>
     <row r="13">
@@ -620,7 +620,7 @@
         <v>111.8992919921875</v>
       </c>
       <c r="D13" t="n">
-        <v>0.01818181818181818</v>
+        <v>0.001771490294322127</v>
       </c>
     </row>
     <row r="14">
@@ -634,7 +634,7 @@
         <v>112.2455368041992</v>
       </c>
       <c r="D14" t="n">
-        <v>0.01666666666666667</v>
+        <v>0.001766074016195434</v>
       </c>
     </row>
     <row r="15">
@@ -648,7 +648,7 @@
         <v>114.1728973388672</v>
       </c>
       <c r="D15" t="n">
-        <v>0.01538461538461539</v>
+        <v>0.001736519655414681</v>
       </c>
     </row>
     <row r="16">
@@ -662,7 +662,7 @@
         <v>130.3114776611328</v>
       </c>
       <c r="D16" t="n">
-        <v>0.01428571428571429</v>
+        <v>0.001523096103724667</v>
       </c>
     </row>
     <row r="17">
@@ -676,7 +676,7 @@
         <v>131.2308349609375</v>
       </c>
       <c r="D17" t="n">
-        <v>0.01333333333333333</v>
+        <v>0.001512506519822569</v>
       </c>
     </row>
     <row r="18">
@@ -690,7 +690,7 @@
         <v>134.7391967773438</v>
       </c>
       <c r="D18" t="n">
-        <v>0.01176470588235294</v>
+        <v>0.001473413757767145</v>
       </c>
     </row>
     <row r="19">
@@ -704,7 +704,7 @@
         <v>136.834716796875</v>
       </c>
       <c r="D19" t="n">
-        <v>0.01111111111111111</v>
+        <v>0.001451013247226655</v>
       </c>
     </row>
     <row r="20">
@@ -718,7 +718,7 @@
         <v>141.8620300292969</v>
       </c>
       <c r="D20" t="n">
-        <v>0.01052631578947368</v>
+        <v>0.001399952107351308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
extra config + calculate overlap
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -457,1276 +457,1276 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2606</v>
+        <v>2580</v>
       </c>
       <c r="B2" t="n">
-        <v>258.01</v>
+        <v>4898.4821</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>22.6196403503418</v>
       </c>
       <c r="D2" t="n">
-        <v>206.408</v>
+        <v>3918.794147529439</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1243</v>
+        <v>1129</v>
       </c>
       <c r="B3" t="n">
-        <v>253.6067</v>
+        <v>4686.8385</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>202.88536</v>
+        <v>3749.4708</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2617</v>
+        <v>878</v>
       </c>
       <c r="B4" t="n">
-        <v>253.5226</v>
+        <v>4573.9623</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>22.86505126953125</v>
       </c>
       <c r="D4" t="n">
-        <v>202.81808</v>
+        <v>3659.178220455493</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>450</v>
+        <v>369</v>
       </c>
       <c r="B5" t="n">
-        <v>251.471</v>
+        <v>4390.2911</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>21.10940551757812</v>
       </c>
       <c r="D5" t="n">
-        <v>201.1768</v>
+        <v>3512.24192592391</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1013</v>
+        <v>1054</v>
       </c>
       <c r="B6" t="n">
-        <v>251.2526</v>
+        <v>4386.5812</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>25.34453773498535</v>
       </c>
       <c r="D6" t="n">
-        <v>201.00208</v>
+        <v>3509.272551706562</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2050</v>
+        <v>1149</v>
       </c>
       <c r="B7" t="n">
-        <v>248.3887</v>
+        <v>4220.5555</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>198.71096</v>
+        <v>3376.4444</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1987</v>
+        <v>2532</v>
       </c>
       <c r="B8" t="n">
-        <v>246.6513</v>
+        <v>4204.0249</v>
       </c>
       <c r="C8" t="n">
-        <v>28.6663990020752</v>
+        <v>22.38754272460938</v>
       </c>
       <c r="D8" t="n">
-        <v>197.3277816338594</v>
+        <v>3363.228471561075</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1400</v>
+        <v>853</v>
       </c>
       <c r="B9" t="n">
-        <v>246.4612</v>
+        <v>4160.4691</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>197.16896</v>
+        <v>3328.37528</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>387</v>
+        <v>1217</v>
       </c>
       <c r="B10" t="n">
-        <v>246.4599</v>
+        <v>4126.5745</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>22.4861888885498</v>
       </c>
       <c r="D10" t="n">
-        <v>197.16792</v>
+        <v>3301.268115642999</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>386</v>
+        <v>1142</v>
       </c>
       <c r="B11" t="n">
-        <v>246.0021</v>
+        <v>4121.5667</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>196.80168</v>
+        <v>3297.253360000001</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1928</v>
+        <v>1144</v>
       </c>
       <c r="B12" t="n">
-        <v>245.5474</v>
+        <v>4111.0639</v>
       </c>
       <c r="C12" t="n">
-        <v>27.62877655029297</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>196.4449059778901</v>
+        <v>3288.85112</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1202</v>
+        <v>1076</v>
       </c>
       <c r="B13" t="n">
-        <v>245.1187</v>
+        <v>4096.3601</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>196.09496</v>
+        <v>3277.08808</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1395</v>
+        <v>1140</v>
       </c>
       <c r="B14" t="n">
-        <v>244.9972</v>
+        <v>4088.1611</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>195.99776</v>
+        <v>3270.52888</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>660</v>
+        <v>1391</v>
       </c>
       <c r="B15" t="n">
-        <v>244.4812</v>
+        <v>4086.7383</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>195.58496</v>
+        <v>3269.39064</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1713</v>
+        <v>2299</v>
       </c>
       <c r="B16" t="n">
-        <v>244.2142</v>
+        <v>4086.7383</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>195.37136</v>
+        <v>3269.39064</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>2456</v>
+        <v>1223</v>
       </c>
       <c r="B17" t="n">
-        <v>244.2142</v>
+        <v>4077.3906</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>195.37136</v>
+        <v>3261.91248</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1225</v>
+        <v>73</v>
       </c>
       <c r="B18" t="n">
-        <v>244.1871</v>
+        <v>4073.794</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>195.34968</v>
+        <v>3259.0352</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>693</v>
+        <v>2201</v>
       </c>
       <c r="B19" t="n">
-        <v>243.7667</v>
+        <v>4062.4037</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>195.01336</v>
+        <v>3249.92296</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>2605</v>
+        <v>1161</v>
       </c>
       <c r="B20" t="n">
-        <v>243.7529</v>
+        <v>4053.4926</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>195.00232</v>
+        <v>3242.79408</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1237</v>
+        <v>2305</v>
       </c>
       <c r="B21" t="n">
-        <v>243.6241</v>
+        <v>4049.3602</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>194.89928</v>
+        <v>3239.48816</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1269</v>
+        <v>1397</v>
       </c>
       <c r="B22" t="n">
-        <v>243.4369</v>
+        <v>4049.3602</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>194.74952</v>
+        <v>3239.48816</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1263</v>
+        <v>2273</v>
       </c>
       <c r="B23" t="n">
-        <v>242.7369</v>
+        <v>4042.2495</v>
       </c>
       <c r="C23" t="n">
-        <v>28.32521057128906</v>
+        <v>23.43802642822266</v>
       </c>
       <c r="D23" t="n">
-        <v>194.1963400703799</v>
+        <v>3233.807783966925</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>281</v>
+        <v>1365</v>
       </c>
       <c r="B24" t="n">
-        <v>242.5715</v>
+        <v>4042.2495</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>23.43802642822266</v>
       </c>
       <c r="D24" t="n">
-        <v>194.0572</v>
+        <v>3233.807783966925</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>211</v>
+        <v>310</v>
       </c>
       <c r="B25" t="n">
-        <v>242.3987</v>
+        <v>4038.7937</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>193.91896</v>
+        <v>3231.03496</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1568</v>
+        <v>554</v>
       </c>
       <c r="B26" t="n">
-        <v>241.9762</v>
+        <v>4030.9431</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>193.58096</v>
+        <v>3224.75448</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>2527</v>
+        <v>1562</v>
       </c>
       <c r="B27" t="n">
-        <v>241.9701</v>
+        <v>4029.3202</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>193.57608</v>
+        <v>3223.45616</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>210</v>
+        <v>322</v>
       </c>
       <c r="B28" t="n">
-        <v>241.9431</v>
+        <v>4024.485</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>193.55448</v>
+        <v>3219.588</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1006</v>
+        <v>1349</v>
       </c>
       <c r="B29" t="n">
-        <v>241.8713</v>
+        <v>4008.7697</v>
       </c>
       <c r="C29" t="n">
-        <v>26.40854644775391</v>
+        <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>193.5043369940373</v>
+        <v>3207.01576</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1285</v>
+        <v>2257</v>
       </c>
       <c r="B30" t="n">
-        <v>241.807</v>
+        <v>4008.7697</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>193.4456</v>
+        <v>3207.01576</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>2296</v>
+        <v>1416</v>
       </c>
       <c r="B31" t="n">
-        <v>241.7502</v>
+        <v>4004.7671</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>193.40016</v>
+        <v>3203.81368</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>1984</v>
+        <v>2242</v>
       </c>
       <c r="B32" t="n">
-        <v>241.4644</v>
+        <v>4000.4076</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>193.17152</v>
+        <v>3200.32608</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1264</v>
+        <v>1334</v>
       </c>
       <c r="B33" t="n">
-        <v>241.0754</v>
+        <v>4000.4076</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>192.86032</v>
+        <v>3200.32608</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>722</v>
+        <v>713</v>
       </c>
       <c r="B34" t="n">
-        <v>241.0581</v>
+        <v>4000.0431</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>192.84648</v>
+        <v>3200.03448</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>1153</v>
+        <v>2436</v>
       </c>
       <c r="B35" t="n">
-        <v>240.9175</v>
+        <v>4000.0304</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>192.734</v>
+        <v>3200.02432</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1103</v>
+        <v>2034</v>
       </c>
       <c r="B36" t="n">
-        <v>240.6493</v>
+        <v>3994.4244</v>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>28.45861434936523</v>
       </c>
       <c r="D36" t="n">
-        <v>192.51944</v>
+        <v>3195.546309185589</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1459</v>
+        <v>1153</v>
       </c>
       <c r="B37" t="n">
-        <v>240.5994</v>
+        <v>3992.6468</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>192.47952</v>
+        <v>3194.11744</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>64</v>
+        <v>1157</v>
       </c>
       <c r="B38" t="n">
-        <v>240.5919</v>
+        <v>3992.0688</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>192.47352</v>
+        <v>3193.65504</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>1009</v>
+        <v>537</v>
       </c>
       <c r="B39" t="n">
-        <v>240.5873</v>
+        <v>3991.0569</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>192.46984</v>
+        <v>3192.84552</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>685</v>
+        <v>1480</v>
       </c>
       <c r="B40" t="n">
-        <v>240.3475</v>
+        <v>3986.918</v>
       </c>
       <c r="C40" t="n">
-        <v>28.56905746459961</v>
+        <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>192.2847638273638</v>
+        <v>3189.5344</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1577</v>
+        <v>1158</v>
       </c>
       <c r="B41" t="n">
-        <v>197.10055</v>
+        <v>3984.6652</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>157.68044</v>
+        <v>3187.73216</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>1040</v>
+        <v>1233</v>
       </c>
       <c r="B42" t="n">
-        <v>193.8813</v>
+        <v>3984.1298</v>
       </c>
       <c r="C42" t="n">
-        <v>29.52682018280029</v>
+        <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>155.1115916158841</v>
+        <v>3187.30384</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>1951</v>
+        <v>1904</v>
       </c>
       <c r="B43" t="n">
-        <v>193.2711</v>
+        <v>3983.7207</v>
       </c>
       <c r="C43" t="n">
-        <v>29.04455375671387</v>
+        <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>154.623536780514</v>
+        <v>3186.97656</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>690</v>
+        <v>2081</v>
       </c>
       <c r="B44" t="n">
-        <v>191.9605</v>
+        <v>3983.1512</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>153.5684</v>
+        <v>3186.52096</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>1985</v>
+        <v>1227</v>
       </c>
       <c r="B45" t="n">
-        <v>191.8514</v>
+        <v>3982.7664</v>
       </c>
       <c r="C45" t="n">
-        <v>32.33624458312988</v>
+        <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>153.4871194760208</v>
+        <v>3186.21312</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>403</v>
+        <v>1572</v>
       </c>
       <c r="B46" t="n">
-        <v>190.0211</v>
+        <v>3982.3266</v>
       </c>
       <c r="C46" t="n">
-        <v>29.92715263366699</v>
+        <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>152.0233468093558</v>
+        <v>3185.86128</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>2049</v>
+        <v>628</v>
       </c>
       <c r="B47" t="n">
-        <v>189.94505</v>
+        <v>3982.0065</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>151.95604</v>
+        <v>3185.6052</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>1165</v>
+        <v>1066</v>
       </c>
       <c r="B48" t="n">
-        <v>188.5868</v>
+        <v>3979.2238</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>150.86944</v>
+        <v>3183.37904</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>1559</v>
+        <v>1734</v>
       </c>
       <c r="B49" t="n">
-        <v>187.9899</v>
+        <v>3976.7554</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>150.39192</v>
+        <v>3181.40432</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>1204</v>
+        <v>2105</v>
       </c>
       <c r="B50" t="n">
-        <v>187.7199</v>
+        <v>3976.685</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>150.17592</v>
+        <v>3181.348</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>1192</v>
+        <v>544</v>
       </c>
       <c r="B51" t="n">
-        <v>187.14005</v>
+        <v>3976.2315</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>149.71204</v>
+        <v>3180.9852</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>1952</v>
+        <v>2172</v>
       </c>
       <c r="B52" t="n">
         <v>0</v>
       </c>
       <c r="C52" t="n">
-        <v>25.58623695373535</v>
+        <v>24.87474250793457</v>
       </c>
       <c r="D52" t="n">
-        <v>0.007522689290253246</v>
+        <v>0.007729545518710742</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>1947</v>
+        <v>2169</v>
       </c>
       <c r="B53" t="n">
         <v>0</v>
       </c>
       <c r="C53" t="n">
-        <v>25.8963508605957</v>
+        <v>24.91284561157227</v>
       </c>
       <c r="D53" t="n">
-        <v>0.007435952967620173</v>
+        <v>0.007718179739807625</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>1008</v>
+        <v>1240</v>
       </c>
       <c r="B54" t="n">
         <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>26.15267944335938</v>
+        <v>25.18361282348633</v>
       </c>
       <c r="D54" t="n">
-        <v>0.007365755575511471</v>
+        <v>0.007638365314529966</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>1949</v>
+        <v>2181</v>
       </c>
       <c r="B55" t="n">
         <v>0</v>
       </c>
       <c r="C55" t="n">
-        <v>26.74845504760742</v>
+        <v>25.71427345275879</v>
       </c>
       <c r="D55" t="n">
-        <v>0.007207608483314272</v>
+        <v>0.007486634452315452</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>2405</v>
+        <v>324</v>
       </c>
       <c r="B56" t="n">
         <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>27.08899879455566</v>
+        <v>26.23634719848633</v>
       </c>
       <c r="D56" t="n">
-        <v>0.007120225304675683</v>
+        <v>0.007343128597329495</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>2206</v>
+        <v>2171</v>
       </c>
       <c r="B57" t="n">
         <v>0</v>
       </c>
       <c r="C57" t="n">
-        <v>27.09107208251953</v>
+        <v>26.4426155090332</v>
       </c>
       <c r="D57" t="n">
-        <v>0.007119699789758316</v>
+        <v>0.007287935070699314</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>588</v>
+        <v>1829</v>
       </c>
       <c r="B58" t="n">
         <v>0</v>
       </c>
       <c r="C58" t="n">
-        <v>27.40373039245605</v>
+        <v>27.18692779541016</v>
       </c>
       <c r="D58" t="n">
-        <v>0.007041328629605617</v>
+        <v>0.007095487718692322</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>2317</v>
+        <v>337</v>
       </c>
       <c r="B59" t="n">
         <v>0</v>
       </c>
       <c r="C59" t="n">
-        <v>28.01416015625</v>
+        <v>27.26460456848145</v>
       </c>
       <c r="D59" t="n">
-        <v>0.00689318591070497</v>
+        <v>0.007075987902658469</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>209</v>
+        <v>2173</v>
       </c>
       <c r="B60" t="n">
         <v>0</v>
       </c>
       <c r="C60" t="n">
-        <v>28.16336822509766</v>
+        <v>27.59487915039062</v>
       </c>
       <c r="D60" t="n">
-        <v>0.00685791841519466</v>
+        <v>0.00699425931993379</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>1909</v>
+        <v>2112</v>
       </c>
       <c r="B61" t="n">
         <v>0</v>
       </c>
       <c r="C61" t="n">
-        <v>28.56754684448242</v>
+        <v>27.746826171875</v>
       </c>
       <c r="D61" t="n">
-        <v>0.006764172930948509</v>
+        <v>0.006957289782329911</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>2223</v>
+        <v>2113</v>
       </c>
       <c r="B62" t="n">
         <v>0</v>
       </c>
       <c r="C62" t="n">
-        <v>28.73993492126465</v>
+        <v>27.88826370239258</v>
       </c>
       <c r="D62" t="n">
-        <v>0.006724964278822143</v>
+        <v>0.006923226749118732</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>178</v>
+        <v>2178</v>
       </c>
       <c r="B63" t="n">
         <v>0</v>
       </c>
       <c r="C63" t="n">
-        <v>28.80181121826172</v>
+        <v>28.13891983032227</v>
       </c>
       <c r="D63" t="n">
-        <v>0.00671100150709785</v>
+        <v>0.006863672406685367</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>1405</v>
+        <v>55</v>
       </c>
       <c r="B64" t="n">
         <v>0</v>
       </c>
       <c r="C64" t="n">
-        <v>28.85651588439941</v>
+        <v>28.14017105102539</v>
       </c>
       <c r="D64" t="n">
-        <v>0.006698705259996655</v>
+        <v>0.006863377694310492</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>1925</v>
+        <v>1849</v>
       </c>
       <c r="B65" t="n">
         <v>0</v>
       </c>
       <c r="C65" t="n">
-        <v>28.96027946472168</v>
+        <v>28.23993110656738</v>
       </c>
       <c r="D65" t="n">
-        <v>0.006675505154599796</v>
+        <v>0.006839961396320779</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>119</v>
+        <v>1109</v>
       </c>
       <c r="B66" t="n">
         <v>0</v>
       </c>
       <c r="C66" t="n">
-        <v>29.0321044921875</v>
+        <v>28.27017211914062</v>
       </c>
       <c r="D66" t="n">
-        <v>0.006659539961710897</v>
+        <v>0.006832894565359052</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>2362</v>
+        <v>1854</v>
       </c>
       <c r="B67" t="n">
         <v>0</v>
       </c>
       <c r="C67" t="n">
-        <v>29.12216567993164</v>
+        <v>28.4127311706543</v>
       </c>
       <c r="D67" t="n">
-        <v>0.006639628840938435</v>
+        <v>0.006799776560686899</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>1406</v>
+        <v>2108</v>
       </c>
       <c r="B68" t="n">
         <v>0</v>
       </c>
       <c r="C68" t="n">
-        <v>29.21059417724609</v>
+        <v>28.47624015808105</v>
       </c>
       <c r="D68" t="n">
-        <v>0.006620194188389559</v>
+        <v>0.006785125881978167</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>593</v>
+        <v>339</v>
       </c>
       <c r="B69" t="n">
         <v>0</v>
       </c>
       <c r="C69" t="n">
-        <v>29.30745315551758</v>
+        <v>28.65564918518066</v>
       </c>
       <c r="D69" t="n">
-        <v>0.006599036843304972</v>
+        <v>0.00674407762079755</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>1081</v>
+        <v>638</v>
       </c>
       <c r="B70" t="n">
         <v>0</v>
       </c>
       <c r="C70" t="n">
-        <v>29.30863380432129</v>
+        <v>28.65979766845703</v>
       </c>
       <c r="D70" t="n">
-        <v>0.006598779783055901</v>
+        <v>0.0067431343340787</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>468</v>
+        <v>635</v>
       </c>
       <c r="B71" t="n">
         <v>0</v>
       </c>
       <c r="C71" t="n">
-        <v>29.42081832885742</v>
+        <v>28.67305374145508</v>
       </c>
       <c r="D71" t="n">
-        <v>0.006574445099995174</v>
+        <v>0.006740121921478804</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>411</v>
+        <v>2170</v>
       </c>
       <c r="B72" t="n">
         <v>0</v>
       </c>
       <c r="C72" t="n">
-        <v>29.47954940795898</v>
+        <v>28.81633758544922</v>
       </c>
       <c r="D72" t="n">
-        <v>0.006561776794107558</v>
+        <v>0.006707731941484414</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>58</v>
+        <v>2573</v>
       </c>
       <c r="B73" t="n">
         <v>0</v>
       </c>
       <c r="C73" t="n">
-        <v>29.49860572814941</v>
+        <v>28.97299385070801</v>
       </c>
       <c r="D73" t="n">
-        <v>0.006557676825711585</v>
+        <v>0.006672673440503699</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>1942</v>
+        <v>639</v>
       </c>
       <c r="B74" t="n">
         <v>0</v>
       </c>
       <c r="C74" t="n">
-        <v>31.45183753967285</v>
+        <v>29.17927551269531</v>
       </c>
       <c r="D74" t="n">
-        <v>0.006162979207433078</v>
+        <v>0.006627064321536391</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>1937</v>
+        <v>1110</v>
       </c>
       <c r="B75" t="n">
         <v>0</v>
       </c>
       <c r="C75" t="n">
-        <v>32.34757041931152</v>
+        <v>29.24186325073242</v>
       </c>
       <c r="D75" t="n">
-        <v>0.005997438418607562</v>
+        <v>0.006613349129378008</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>1941</v>
+        <v>995</v>
       </c>
       <c r="B76" t="n">
         <v>0</v>
       </c>
       <c r="C76" t="n">
-        <v>32.85299587249756</v>
+        <v>29.2713623046875</v>
       </c>
       <c r="D76" t="n">
-        <v>0.005907896623190197</v>
+        <v>0.006606904505550785</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>2013</v>
+        <v>2110</v>
       </c>
       <c r="B77" t="n">
         <v>0</v>
       </c>
       <c r="C77" t="n">
-        <v>33.26922035217285</v>
+        <v>29.27565765380859</v>
       </c>
       <c r="D77" t="n">
-        <v>0.005836140943525111</v>
+        <v>0.006605967153114527</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>1584</v>
+        <v>2063</v>
       </c>
       <c r="B78" t="n">
         <v>0</v>
       </c>
       <c r="C78" t="n">
-        <v>33.58369827270508</v>
+        <v>29.29341506958008</v>
       </c>
       <c r="D78" t="n">
-        <v>0.005783071504468003</v>
+        <v>0.006602094862551012</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>1986</v>
+        <v>2274</v>
       </c>
       <c r="B79" t="n">
         <v>0</v>
       </c>
       <c r="C79" t="n">
-        <v>33.63115119934082</v>
+        <v>29.33083343505859</v>
       </c>
       <c r="D79" t="n">
-        <v>0.005775147318920397</v>
+        <v>0.006593950028713204</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>56</v>
+        <v>1366</v>
       </c>
       <c r="B80" t="n">
         <v>0</v>
       </c>
       <c r="C80" t="n">
-        <v>33.77913951873779</v>
+        <v>29.33083343505859</v>
       </c>
       <c r="D80" t="n">
-        <v>0.005750573555514418</v>
+        <v>0.006593950028713204</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>181</v>
+        <v>2667</v>
       </c>
       <c r="B81" t="n">
         <v>0</v>
       </c>
       <c r="C81" t="n">
-        <v>33.88164043426514</v>
+        <v>29.35636520385742</v>
       </c>
       <c r="D81" t="n">
-        <v>0.005733675294798775</v>
+        <v>0.00658840406803993</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>1267</v>
+        <v>2179</v>
       </c>
       <c r="B82" t="n">
         <v>0</v>
       </c>
       <c r="C82" t="n">
-        <v>34.30237483978271</v>
+        <v>29.3653507232666</v>
       </c>
       <c r="D82" t="n">
-        <v>0.005665341238590481</v>
+        <v>0.006586454469855854</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>748</v>
+        <v>2592</v>
       </c>
       <c r="B83" t="n">
         <v>0</v>
       </c>
       <c r="C83" t="n">
-        <v>34.46516513824463</v>
+        <v>29.42089462280273</v>
       </c>
       <c r="D83" t="n">
-        <v>0.005639336493158626</v>
+        <v>0.006574428611645269</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>511</v>
+        <v>630</v>
       </c>
       <c r="B84" t="n">
         <v>0</v>
       </c>
       <c r="C84" t="n">
-        <v>34.58765602111816</v>
+        <v>29.46918869018555</v>
       </c>
       <c r="D84" t="n">
-        <v>0.005619926186802454</v>
+        <v>0.006564008055272643</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>1933</v>
+        <v>315</v>
       </c>
       <c r="B85" t="n">
         <v>0</v>
       </c>
       <c r="C85" t="n">
-        <v>34.74050807952881</v>
+        <v>29.55693054199219</v>
       </c>
       <c r="D85" t="n">
-        <v>0.00559589134980861</v>
+        <v>0.006545160016159163</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>2315</v>
+        <v>637</v>
       </c>
       <c r="B86" t="n">
         <v>0</v>
       </c>
       <c r="C86" t="n">
-        <v>34.82036685943604</v>
+        <v>29.57680130004883</v>
       </c>
       <c r="D86" t="n">
-        <v>0.005583415736215853</v>
+        <v>0.006540906553220158</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>2408</v>
+        <v>2175</v>
       </c>
       <c r="B87" t="n">
         <v>0</v>
       </c>
       <c r="C87" t="n">
-        <v>35.08691215515137</v>
+        <v>29.60577392578125</v>
       </c>
       <c r="D87" t="n">
-        <v>0.005542175488446446</v>
+        <v>0.006534714674590433</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>2441</v>
+        <v>335</v>
       </c>
       <c r="B88" t="n">
         <v>0</v>
       </c>
       <c r="C88" t="n">
-        <v>35.16096591949463</v>
+        <v>29.65115737915039</v>
       </c>
       <c r="D88" t="n">
-        <v>0.005530825709834776</v>
+        <v>0.00652503908828071</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>1698</v>
+        <v>336</v>
       </c>
       <c r="B89" t="n">
         <v>0</v>
       </c>
       <c r="C89" t="n">
-        <v>35.16096591949463</v>
+        <v>29.66428756713867</v>
       </c>
       <c r="D89" t="n">
-        <v>0.005530825709834776</v>
+        <v>0.006522245121857312</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>356</v>
+        <v>1851</v>
       </c>
       <c r="B90" t="n">
         <v>0</v>
       </c>
       <c r="C90" t="n">
-        <v>35.40172958374023</v>
+        <v>29.66816139221191</v>
       </c>
       <c r="D90" t="n">
-        <v>0.005494244429784873</v>
+        <v>0.006521421269512081</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>681</v>
+        <v>1114</v>
       </c>
       <c r="B91" t="n">
         <v>0</v>
       </c>
       <c r="C91" t="n">
-        <v>35.5405158996582</v>
+        <v>29.73601913452148</v>
       </c>
       <c r="D91" t="n">
-        <v>0.005473376472001885</v>
+        <v>0.006507023538886592</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>213</v>
+        <v>1112</v>
       </c>
       <c r="B92" t="n">
         <v>0</v>
       </c>
       <c r="C92" t="n">
-        <v>35.78712272644043</v>
+        <v>29.80475044250488</v>
       </c>
       <c r="D92" t="n">
-        <v>0.005436685045668215</v>
+        <v>0.006492505121029542</v>
       </c>
     </row>
   </sheetData>

</xml_diff>